<commit_message>
Updated existing steps and methods, added screenshot capability in structured way for failure cases
</commit_message>
<xml_diff>
--- a/cucumber-for-appian/src/test/resources/testdata/01_SMB_End2End.xlsx
+++ b/cucumber-for-appian/src/test/resources/testdata/01_SMB_End2End.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\IdeaProjects\ORIXAutoExcel\cucumber-for-appian\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0B9B08-2BD2-46D6-8EBD-6659BB4AB5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751961AA-E222-43D8-8907-F901489BA2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="873" xr2:uid="{25A2403C-A232-4567-AEA7-838C07E97658}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="258">
   <si>
     <t>Passenger cars including electric vehicles</t>
   </si>
@@ -703,9 +703,6 @@
     <t>D:\ORIX_AUS\UploadDocs\Financial_Statement_Document.pdf</t>
   </si>
   <si>
-    <t>No[7]</t>
-  </si>
-  <si>
     <t>Rental Agreement</t>
   </si>
   <si>
@@ -776,36 +773,83 @@
     <t>$1,411.34</t>
   </si>
   <si>
-    <t>APP-615</t>
-  </si>
-  <si>
-    <t>SMB-00000889
-SMB-00000889</t>
-  </si>
-  <si>
-    <t>03 Feb 2026 09:01 PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Planting equipment</t>
-  </si>
-  <si>
-    <t>APP-616</t>
-  </si>
-  <si>
-    <t>SMB-00000890
-SMB-00000890</t>
-  </si>
-  <si>
-    <t>03 Feb 2026 09:07 PM</t>
-  </si>
-  <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>APP-659</t>
+  </si>
+  <si>
+    <t>SMB-00000952
+SMB-00000952</t>
+  </si>
+  <si>
+    <t>11 Feb 2026 03:51 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Medium and heavy co... more</t>
+  </si>
+  <si>
+    <t>APP-663</t>
+  </si>
+  <si>
+    <t>SMB-00000960
+SMB-00000960</t>
+  </si>
+  <si>
+    <t>11 Feb 2026 05:50 PM</t>
+  </si>
+  <si>
+    <t>No[7]</t>
+  </si>
+  <si>
+    <t>APP-664</t>
+  </si>
+  <si>
+    <t>SMB-00000962
+SMB-00000962</t>
+  </si>
+  <si>
+    <t>11 Feb 2026 06:22 PM</t>
+  </si>
+  <si>
+    <t>APP-665</t>
+  </si>
+  <si>
+    <t>SMB-00000963
+SMB-00000963</t>
+  </si>
+  <si>
+    <t>11 Feb 2026 06:25 PM</t>
+  </si>
+  <si>
+    <t>APP-673</t>
+  </si>
+  <si>
+    <t>SMB-00000974
+SMB-00000974</t>
+  </si>
+  <si>
+    <t>11 Feb 2026 08:50 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FORD MUSTANG </t>
+  </si>
+  <si>
+    <t>APP-674</t>
+  </si>
+  <si>
+    <t>SMB-00000975
+SMB-00000975</t>
+  </si>
+  <si>
+    <t>11 Feb 2026 08:55 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1284,95 +1328,95 @@
   <dimension ref="A1:DO25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CZ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DA1" sqref="DA1"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="4.21875" customWidth="1"/>
-    <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" customWidth="1"/>
-    <col min="11" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" customWidth="1"/>
-    <col min="16" max="16" width="10.88671875" customWidth="1"/>
-    <col min="17" max="17" width="14.5546875" customWidth="1"/>
-    <col min="18" max="18" width="6.88671875" customWidth="1"/>
-    <col min="19" max="19" width="5.77734375" customWidth="1"/>
-    <col min="20" max="20" width="6.77734375" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="24" max="24" width="9.109375" customWidth="1"/>
-    <col min="25" max="25" width="11" customWidth="1"/>
-    <col min="26" max="26" width="8.88671875" customWidth="1"/>
-    <col min="27" max="34" width="6.5546875" customWidth="1"/>
-    <col min="35" max="35" width="7.6640625" customWidth="1"/>
-    <col min="37" max="37" width="8.5546875" customWidth="1"/>
-    <col min="38" max="39" width="8.44140625" customWidth="1"/>
-    <col min="40" max="40" width="10.5546875" customWidth="1"/>
-    <col min="41" max="41" width="10" customWidth="1"/>
-    <col min="43" max="43" width="6.33203125" customWidth="1"/>
-    <col min="44" max="44" width="14.5546875" customWidth="1"/>
-    <col min="45" max="45" width="6.88671875" customWidth="1"/>
-    <col min="46" max="46" width="5.77734375" customWidth="1"/>
-    <col min="47" max="47" width="7.88671875" customWidth="1"/>
-    <col min="48" max="48" width="9.88671875" customWidth="1"/>
-    <col min="49" max="49" width="8.44140625" customWidth="1"/>
-    <col min="50" max="52" width="12.109375" customWidth="1"/>
-    <col min="53" max="53" width="13.6640625" customWidth="1"/>
-    <col min="54" max="54" width="15.33203125" customWidth="1"/>
-    <col min="55" max="55" width="21.33203125" customWidth="1"/>
-    <col min="56" max="56" width="12.44140625" customWidth="1"/>
-    <col min="57" max="57" width="15.88671875" customWidth="1"/>
-    <col min="58" max="58" width="21.44140625" customWidth="1"/>
-    <col min="59" max="59" width="18.6640625" customWidth="1"/>
-    <col min="60" max="60" width="18.33203125" customWidth="1"/>
-    <col min="61" max="61" width="19.109375" customWidth="1"/>
-    <col min="62" max="62" width="7.21875" customWidth="1"/>
-    <col min="63" max="63" width="7.77734375" customWidth="1"/>
-    <col min="64" max="64" width="12.6640625" customWidth="1"/>
-    <col min="65" max="65" width="10.109375" customWidth="1"/>
-    <col min="66" max="66" width="11.88671875" customWidth="1"/>
-    <col min="67" max="67" width="7.6640625" customWidth="1"/>
-    <col min="68" max="68" width="10.33203125" customWidth="1"/>
-    <col min="69" max="69" width="10.109375" customWidth="1"/>
-    <col min="70" max="70" width="12" customWidth="1"/>
-    <col min="71" max="71" width="12.109375" customWidth="1"/>
-    <col min="72" max="72" width="8.6640625" customWidth="1"/>
-    <col min="73" max="73" width="10.109375" customWidth="1"/>
-    <col min="74" max="74" width="9.21875" customWidth="1"/>
-    <col min="75" max="75" width="12.109375" customWidth="1"/>
-    <col min="76" max="76" width="13.5546875" customWidth="1"/>
-    <col min="77" max="77" width="10.109375" customWidth="1"/>
-    <col min="78" max="79" width="23.109375" customWidth="1"/>
-    <col min="80" max="80" width="7.44140625" customWidth="1"/>
-    <col min="81" max="81" width="10.33203125" customWidth="1"/>
-    <col min="82" max="82" width="8.5546875" customWidth="1"/>
-    <col min="83" max="83" width="9.6640625" customWidth="1"/>
-    <col min="84" max="84" width="13.6640625" customWidth="1"/>
-    <col min="85" max="85" width="11.109375" customWidth="1"/>
-    <col min="86" max="86" width="14.6640625" customWidth="1"/>
-    <col min="87" max="87" width="28.44140625" customWidth="1"/>
-    <col min="88" max="88" width="25.6640625" customWidth="1"/>
-    <col min="89" max="89" width="14.6640625" customWidth="1"/>
-    <col min="90" max="90" width="32.109375" customWidth="1"/>
-    <col min="91" max="103" width="14.6640625" customWidth="1"/>
-    <col min="104" max="104" width="9.21875" customWidth="1"/>
-    <col min="105" max="105" width="6.21875" customWidth="1"/>
-    <col min="106" max="118" width="14.6640625" customWidth="1"/>
-    <col min="119" max="119" width="27" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="9.109375"/>
+    <col min="2" max="2" customWidth="true" width="11.0"/>
+    <col min="3" max="3" customWidth="true" width="16.88671875"/>
+    <col min="4" max="4" customWidth="true" width="4.21875"/>
+    <col min="5" max="5" customWidth="true" width="7.0"/>
+    <col min="6" max="6" customWidth="true" width="16.33203125"/>
+    <col min="7" max="7" customWidth="true" width="12.77734375"/>
+    <col min="8" max="8" customWidth="true" width="16.33203125"/>
+    <col min="9" max="9" customWidth="true" width="9.77734375"/>
+    <col min="10" max="10" customWidth="true" width="19.33203125"/>
+    <col min="11" max="12" customWidth="true" width="8.44140625"/>
+    <col min="13" max="13" customWidth="true" width="9.5546875"/>
+    <col min="14" max="14" customWidth="true" width="17.5546875"/>
+    <col min="15" max="15" customWidth="true" width="10.77734375"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875"/>
+    <col min="17" max="17" customWidth="true" width="14.5546875"/>
+    <col min="18" max="18" customWidth="true" width="6.88671875"/>
+    <col min="19" max="19" customWidth="true" width="5.77734375"/>
+    <col min="20" max="20" customWidth="true" width="6.77734375"/>
+    <col min="21" max="21" customWidth="true" width="12.6640625"/>
+    <col min="22" max="22" customWidth="true" width="8.33203125"/>
+    <col min="23" max="23" customWidth="true" width="11.6640625"/>
+    <col min="24" max="24" customWidth="true" width="9.109375"/>
+    <col min="25" max="25" customWidth="true" width="11.0"/>
+    <col min="26" max="26" customWidth="true" width="8.88671875"/>
+    <col min="27" max="34" customWidth="true" width="6.5546875"/>
+    <col min="35" max="35" customWidth="true" width="7.6640625"/>
+    <col min="37" max="37" customWidth="true" width="8.5546875"/>
+    <col min="38" max="39" customWidth="true" width="8.44140625"/>
+    <col min="40" max="40" customWidth="true" width="10.5546875"/>
+    <col min="41" max="41" customWidth="true" width="10.0"/>
+    <col min="43" max="43" customWidth="true" width="6.33203125"/>
+    <col min="44" max="44" customWidth="true" width="14.5546875"/>
+    <col min="45" max="45" customWidth="true" width="6.88671875"/>
+    <col min="46" max="46" customWidth="true" width="5.77734375"/>
+    <col min="47" max="47" customWidth="true" width="7.88671875"/>
+    <col min="48" max="48" customWidth="true" width="9.88671875"/>
+    <col min="49" max="49" customWidth="true" width="8.44140625"/>
+    <col min="50" max="52" customWidth="true" width="12.109375"/>
+    <col min="53" max="53" customWidth="true" width="13.6640625"/>
+    <col min="54" max="54" customWidth="true" width="15.33203125"/>
+    <col min="55" max="55" customWidth="true" width="21.33203125"/>
+    <col min="56" max="56" customWidth="true" width="12.44140625"/>
+    <col min="57" max="57" customWidth="true" width="15.88671875"/>
+    <col min="58" max="58" customWidth="true" width="21.44140625"/>
+    <col min="59" max="59" customWidth="true" width="18.6640625"/>
+    <col min="60" max="60" customWidth="true" width="18.33203125"/>
+    <col min="61" max="61" customWidth="true" width="19.109375"/>
+    <col min="62" max="62" customWidth="true" width="7.21875"/>
+    <col min="63" max="63" customWidth="true" width="7.77734375"/>
+    <col min="64" max="64" customWidth="true" width="12.6640625"/>
+    <col min="65" max="65" customWidth="true" width="10.109375"/>
+    <col min="66" max="66" customWidth="true" width="11.88671875"/>
+    <col min="67" max="67" customWidth="true" width="7.6640625"/>
+    <col min="68" max="68" customWidth="true" width="10.33203125"/>
+    <col min="69" max="69" customWidth="true" width="10.109375"/>
+    <col min="70" max="70" customWidth="true" width="12.0"/>
+    <col min="71" max="71" customWidth="true" width="12.109375"/>
+    <col min="72" max="72" customWidth="true" width="8.6640625"/>
+    <col min="73" max="73" customWidth="true" width="10.109375"/>
+    <col min="74" max="74" customWidth="true" width="9.21875"/>
+    <col min="75" max="75" customWidth="true" width="12.109375"/>
+    <col min="76" max="76" customWidth="true" width="13.5546875"/>
+    <col min="77" max="77" customWidth="true" width="10.109375"/>
+    <col min="78" max="79" customWidth="true" width="23.109375"/>
+    <col min="80" max="80" customWidth="true" width="7.44140625"/>
+    <col min="81" max="81" customWidth="true" width="10.33203125"/>
+    <col min="82" max="82" customWidth="true" width="8.5546875"/>
+    <col min="83" max="83" customWidth="true" width="9.6640625"/>
+    <col min="84" max="84" customWidth="true" width="13.6640625"/>
+    <col min="85" max="85" customWidth="true" width="11.109375"/>
+    <col min="86" max="86" customWidth="true" width="14.6640625"/>
+    <col min="87" max="87" customWidth="true" width="28.44140625"/>
+    <col min="88" max="88" customWidth="true" width="25.6640625"/>
+    <col min="89" max="89" customWidth="true" width="14.6640625"/>
+    <col min="90" max="90" customWidth="true" width="32.109375"/>
+    <col min="91" max="103" customWidth="true" width="14.6640625"/>
+    <col min="104" max="104" customWidth="true" width="9.21875"/>
+    <col min="105" max="105" customWidth="true" width="6.21875"/>
+    <col min="106" max="118" customWidth="true" width="14.6640625"/>
+    <col min="119" max="119" customWidth="true" width="27.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:119" s="3" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
@@ -1629,16 +1673,16 @@
         <v>140</v>
       </c>
       <c r="CG1" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="CH1" s="2" t="s">
         <v>71</v>
       </c>
       <c r="CI1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CJ1" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="CJ1" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="CK1" s="2" t="s">
         <v>108</v>
@@ -1677,13 +1721,13 @@
         <v>150</v>
       </c>
       <c r="CW1" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="CX1" s="2" t="s">
         <v>151</v>
       </c>
       <c r="CY1" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="CZ1" s="2" t="s">
         <v>152</v>
@@ -1707,7 +1751,7 @@
         <v>161</v>
       </c>
       <c r="DG1" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="DH1" s="2" t="s">
         <v>163</v>
@@ -1725,13 +1769,13 @@
         <v>170</v>
       </c>
       <c r="DM1" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DN1" s="2" t="s">
         <v>171</v>
       </c>
       <c r="DO1" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:119" s="6" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
@@ -1949,10 +1993,10 @@
         <v>109</v>
       </c>
       <c r="CL2" s="4" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="CM2" s="4" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="CN2" s="4" t="s">
         <v>24</v>
@@ -1961,7 +2005,7 @@
         <v>137</v>
       </c>
       <c r="CP2" s="4" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="CQ2" s="4" t="s">
         <v>174</v>
@@ -2055,7 +2099,7 @@
         <v>77</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="X3" s="4" t="s">
         <v>13</v>
@@ -2236,11 +2280,11 @@
         <v>149</v>
       </c>
       <c r="CV3" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="CW3" s="9"/>
       <c r="CX3" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="CY3" s="9"/>
       <c r="CZ3" s="9" t="s">
@@ -2311,7 +2355,7 @@
         <v>79</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>86</v>
@@ -2330,7 +2374,7 @@
         <v>208</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>195</v>
@@ -2507,10 +2551,10 @@
         <v>196</v>
       </c>
       <c r="CF4" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="CG4" s="11" t="s">
         <v>218</v>
-      </c>
-      <c r="CG4" s="11" t="s">
-        <v>219</v>
       </c>
       <c r="CH4" s="11" t="s">
         <v>82</v>
@@ -2525,10 +2569,10 @@
         <v>109</v>
       </c>
       <c r="CL4" s="4" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="CM4" s="4" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="CN4" s="4" t="s">
         <v>85</v>
@@ -2537,7 +2581,7 @@
         <v>137</v>
       </c>
       <c r="CP4" s="4" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="CQ4" s="4" t="s">
         <v>174</v>
@@ -2645,13 +2689,13 @@
         <v>196</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="V5" s="11" t="s">
         <v>196</v>
       </c>
       <c r="W5" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X5" s="11" t="s">
         <v>13</v>
@@ -2764,7 +2808,7 @@
         <v>91</v>
       </c>
       <c r="BR5" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="BS5" s="11" t="s">
         <v>37</v>
@@ -2802,10 +2846,10 @@
         <v>196</v>
       </c>
       <c r="CF5" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="CG5" s="11" t="s">
         <v>218</v>
-      </c>
-      <c r="CG5" s="11" t="s">
-        <v>219</v>
       </c>
       <c r="CH5" s="11" t="s">
         <v>82</v>
@@ -2832,16 +2876,16 @@
       </c>
       <c r="CS5" s="4"/>
       <c r="CT5" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CU5" s="9"/>
       <c r="CV5" s="9"/>
       <c r="CW5" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CX5" s="9"/>
       <c r="CY5" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="CZ5" s="9" t="s">
         <v>79</v>
@@ -2853,17 +2897,17 @@
         <v>154</v>
       </c>
       <c r="DC5" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="DD5" s="9" t="s">
         <v>192</v>
       </c>
       <c r="DE5" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="DF5" s="9"/>
       <c r="DG5" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="DH5" s="9"/>
       <c r="DI5" s="9" t="s">
@@ -2874,10 +2918,10 @@
       </c>
       <c r="DK5" s="9"/>
       <c r="DL5" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="DM5" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="DN5" s="9"/>
       <c r="DO5" s="4" t="s">

</xml_diff>